<commit_message>
decoration changes in code
</commit_message>
<xml_diff>
--- a/lista_imion_copy.xlsx
+++ b/lista_imion_copy.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView activeTab="1" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-28920" yWindow="-120"/>
+    <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible" windowHeight="15840" windowWidth="29040" xWindow="-120" yWindow="-120"/>
   </bookViews>
   <sheets>
     <sheet name="first names" sheetId="1" state="visible" r:id="rId1"/>
@@ -366,8 +366,8 @@
   </sheetPr>
   <dimension ref="A1:O202"/>
   <sheetViews>
-    <sheetView topLeftCell="A184" workbookViewId="0">
-      <selection activeCell="K200" sqref="K2:K200"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -9470,10 +9470,10 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N1002"/>
+  <dimension ref="A1:H1002"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N10" sqref="N10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -9689,11 +9689,6 @@
         <f>G8+F7</f>
         <v/>
       </c>
-      <c r="N7" t="inlineStr">
-        <is>
-          <t>dupa123</t>
-        </is>
-      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">

</xml_diff>